<commit_message>
fazendo o greety best first com o banco de dados correto
</commit_message>
<xml_diff>
--- a/elementos_do_mapa/planilha_distancias.xlsx
+++ b/elementos_do_mapa/planilha_distancias.xlsx
@@ -20,7 +20,7 @@
     <sheet state="visible" name="Mogi_Mirim" sheetId="15" r:id="rId18"/>
     <sheet state="visible" name="Limeira" sheetId="16" r:id="rId19"/>
     <sheet state="visible" name="Piracicaba" sheetId="17" r:id="rId20"/>
-    <sheet state="visible" name="Itepeva" sheetId="18" r:id="rId21"/>
+    <sheet state="visible" name="Itapeva" sheetId="18" r:id="rId21"/>
     <sheet state="visible" name="Sorocaba" sheetId="19" r:id="rId22"/>
     <sheet state="visible" name="Campinas" sheetId="20" r:id="rId23"/>
     <sheet state="visible" name="Jundiai" sheetId="21" r:id="rId24"/>
@@ -55,7 +55,7 @@
     <t>Marilia</t>
   </si>
   <si>
-    <t xml:space="preserve">Aracatuba </t>
+    <t>Aracatuba</t>
   </si>
   <si>
     <t>Fernandopolis</t>
@@ -79,7 +79,7 @@
     <t>Sao_Carlos</t>
   </si>
   <si>
-    <t xml:space="preserve">Bauru </t>
+    <t>Bauru</t>
   </si>
   <si>
     <t>Botucatu</t>
@@ -97,10 +97,10 @@
     <t>Piracicaba</t>
   </si>
   <si>
-    <t xml:space="preserve">Itapeva </t>
+    <t>Itapeva</t>
   </si>
   <si>
-    <t xml:space="preserve">Sorocaba </t>
+    <t>Sorocaba</t>
   </si>
   <si>
     <t>Campinas</t>
@@ -112,13 +112,13 @@
     <t>SP</t>
   </si>
   <si>
-    <t xml:space="preserve">Guarulhos </t>
+    <t>Guarulhos</t>
   </si>
   <si>
-    <t xml:space="preserve">Registro </t>
+    <t>Registro</t>
   </si>
   <si>
-    <t xml:space="preserve">Itanhaem </t>
+    <t>Itanhaem</t>
   </si>
   <si>
     <t>Santos</t>
@@ -235,7 +235,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="22">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -281,6 +281,9 @@
     <xf borderId="0" fillId="7" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
       <alignment vertical="bottom"/>
     </xf>
+    <xf borderId="0" fillId="7" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0" vertical="bottom"/>
+    </xf>
     <xf borderId="0" fillId="8" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
       <alignment readingOrder="0" vertical="bottom"/>
     </xf>
@@ -288,10 +291,10 @@
       <alignment vertical="bottom"/>
     </xf>
     <xf borderId="0" fillId="9" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
-      <alignment vertical="bottom"/>
+      <alignment readingOrder="0" vertical="bottom"/>
     </xf>
     <xf borderId="0" fillId="9" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" vertical="bottom"/>
+      <alignment vertical="bottom"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" vertical="bottom"/>
@@ -723,7 +726,7 @@
       </c>
     </row>
     <row r="13">
-      <c r="A13" s="11" t="s">
+      <c r="A13" s="10" t="s">
         <v>13</v>
       </c>
       <c r="B13" s="8">
@@ -771,7 +774,7 @@
       </c>
     </row>
     <row r="19">
-      <c r="A19" s="14" t="s">
+      <c r="A19" s="15" t="s">
         <v>19</v>
       </c>
       <c r="B19" s="8">
@@ -779,7 +782,7 @@
       </c>
     </row>
     <row r="20">
-      <c r="A20" s="14" t="s">
+      <c r="A20" s="15" t="s">
         <v>20</v>
       </c>
       <c r="B20" s="8">
@@ -795,7 +798,7 @@
       </c>
     </row>
     <row r="22">
-      <c r="A22" s="15" t="s">
+      <c r="A22" s="16" t="s">
         <v>22</v>
       </c>
       <c r="B22" s="6">
@@ -803,7 +806,7 @@
       </c>
     </row>
     <row r="23">
-      <c r="A23" s="16" t="s">
+      <c r="A23" s="17" t="s">
         <v>23</v>
       </c>
       <c r="B23" s="6">
@@ -827,7 +830,7 @@
       </c>
     </row>
     <row r="26">
-      <c r="A26" s="17" t="s">
+      <c r="A26" s="18" t="s">
         <v>26</v>
       </c>
       <c r="B26" s="8">
@@ -835,7 +838,7 @@
       </c>
     </row>
     <row r="27">
-      <c r="A27" s="17" t="s">
+      <c r="A27" s="19" t="s">
         <v>27</v>
       </c>
       <c r="B27" s="8">
@@ -843,7 +846,7 @@
       </c>
     </row>
     <row r="28">
-      <c r="A28" s="17" t="s">
+      <c r="A28" s="19" t="s">
         <v>28</v>
       </c>
       <c r="B28" s="8">
@@ -873,7 +876,7 @@
   </sheetViews>
   <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
   <cols>
-    <col customWidth="1" min="1" max="1" width="20.75"/>
+    <col customWidth="1" min="1" max="1" width="25.63"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -960,7 +963,7 @@
       <c r="A11" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="B11" s="19">
+      <c r="B11" s="20">
         <v>0.0</v>
       </c>
     </row>
@@ -973,7 +976,7 @@
       </c>
     </row>
     <row r="13">
-      <c r="A13" s="11" t="s">
+      <c r="A13" s="10" t="s">
         <v>13</v>
       </c>
       <c r="B13" s="8">
@@ -1021,7 +1024,7 @@
       </c>
     </row>
     <row r="19">
-      <c r="A19" s="14" t="s">
+      <c r="A19" s="15" t="s">
         <v>19</v>
       </c>
       <c r="B19" s="8">
@@ -1029,7 +1032,7 @@
       </c>
     </row>
     <row r="20">
-      <c r="A20" s="14" t="s">
+      <c r="A20" s="15" t="s">
         <v>20</v>
       </c>
       <c r="B20" s="8">
@@ -1045,7 +1048,7 @@
       </c>
     </row>
     <row r="22">
-      <c r="A22" s="15" t="s">
+      <c r="A22" s="16" t="s">
         <v>22</v>
       </c>
       <c r="B22" s="6">
@@ -1053,7 +1056,7 @@
       </c>
     </row>
     <row r="23">
-      <c r="A23" s="16" t="s">
+      <c r="A23" s="17" t="s">
         <v>23</v>
       </c>
       <c r="B23" s="6">
@@ -1077,7 +1080,7 @@
       </c>
     </row>
     <row r="26">
-      <c r="A26" s="17" t="s">
+      <c r="A26" s="18" t="s">
         <v>26</v>
       </c>
       <c r="B26" s="8">
@@ -1085,7 +1088,7 @@
       </c>
     </row>
     <row r="27">
-      <c r="A27" s="17" t="s">
+      <c r="A27" s="19" t="s">
         <v>27</v>
       </c>
       <c r="B27" s="8">
@@ -1093,7 +1096,7 @@
       </c>
     </row>
     <row r="28">
-      <c r="A28" s="17" t="s">
+      <c r="A28" s="19" t="s">
         <v>28</v>
       </c>
       <c r="B28" s="8">
@@ -1123,7 +1126,7 @@
   </sheetViews>
   <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
   <cols>
-    <col customWidth="1" min="1" max="1" width="20.75"/>
+    <col customWidth="1" min="1" max="1" width="25.63"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -1218,12 +1221,12 @@
       <c r="A12" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="B12" s="19">
+      <c r="B12" s="20">
         <v>0.0</v>
       </c>
     </row>
     <row r="13">
-      <c r="A13" s="11" t="s">
+      <c r="A13" s="10" t="s">
         <v>13</v>
       </c>
       <c r="B13" s="8">
@@ -1271,7 +1274,7 @@
       </c>
     </row>
     <row r="19">
-      <c r="A19" s="14" t="s">
+      <c r="A19" s="15" t="s">
         <v>19</v>
       </c>
       <c r="B19" s="8">
@@ -1279,7 +1282,7 @@
       </c>
     </row>
     <row r="20">
-      <c r="A20" s="14" t="s">
+      <c r="A20" s="15" t="s">
         <v>20</v>
       </c>
       <c r="B20" s="8">
@@ -1295,7 +1298,7 @@
       </c>
     </row>
     <row r="22">
-      <c r="A22" s="15" t="s">
+      <c r="A22" s="16" t="s">
         <v>22</v>
       </c>
       <c r="B22" s="6">
@@ -1303,7 +1306,7 @@
       </c>
     </row>
     <row r="23">
-      <c r="A23" s="16" t="s">
+      <c r="A23" s="17" t="s">
         <v>23</v>
       </c>
       <c r="B23" s="6">
@@ -1327,7 +1330,7 @@
       </c>
     </row>
     <row r="26">
-      <c r="A26" s="17" t="s">
+      <c r="A26" s="18" t="s">
         <v>26</v>
       </c>
       <c r="B26" s="8">
@@ -1335,7 +1338,7 @@
       </c>
     </row>
     <row r="27">
-      <c r="A27" s="17" t="s">
+      <c r="A27" s="19" t="s">
         <v>27</v>
       </c>
       <c r="B27" s="8">
@@ -1343,7 +1346,7 @@
       </c>
     </row>
     <row r="28">
-      <c r="A28" s="17" t="s">
+      <c r="A28" s="19" t="s">
         <v>28</v>
       </c>
       <c r="B28" s="8">
@@ -1373,7 +1376,7 @@
   </sheetViews>
   <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
   <cols>
-    <col customWidth="1" min="1" max="1" width="20.75"/>
+    <col customWidth="1" min="1" max="1" width="25.63"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -1473,10 +1476,10 @@
       </c>
     </row>
     <row r="13">
-      <c r="A13" s="11" t="s">
+      <c r="A13" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="B13" s="19">
+      <c r="B13" s="20">
         <v>0.0</v>
       </c>
     </row>
@@ -1521,7 +1524,7 @@
       </c>
     </row>
     <row r="19">
-      <c r="A19" s="14" t="s">
+      <c r="A19" s="15" t="s">
         <v>19</v>
       </c>
       <c r="B19" s="8">
@@ -1529,7 +1532,7 @@
       </c>
     </row>
     <row r="20">
-      <c r="A20" s="14" t="s">
+      <c r="A20" s="15" t="s">
         <v>20</v>
       </c>
       <c r="B20" s="8">
@@ -1545,7 +1548,7 @@
       </c>
     </row>
     <row r="22">
-      <c r="A22" s="15" t="s">
+      <c r="A22" s="16" t="s">
         <v>22</v>
       </c>
       <c r="B22" s="6">
@@ -1553,7 +1556,7 @@
       </c>
     </row>
     <row r="23">
-      <c r="A23" s="16" t="s">
+      <c r="A23" s="17" t="s">
         <v>23</v>
       </c>
       <c r="B23" s="6">
@@ -1577,7 +1580,7 @@
       </c>
     </row>
     <row r="26">
-      <c r="A26" s="17" t="s">
+      <c r="A26" s="18" t="s">
         <v>26</v>
       </c>
       <c r="B26" s="8">
@@ -1585,7 +1588,7 @@
       </c>
     </row>
     <row r="27">
-      <c r="A27" s="17" t="s">
+      <c r="A27" s="19" t="s">
         <v>27</v>
       </c>
       <c r="B27" s="8">
@@ -1593,7 +1596,7 @@
       </c>
     </row>
     <row r="28">
-      <c r="A28" s="17" t="s">
+      <c r="A28" s="19" t="s">
         <v>28</v>
       </c>
       <c r="B28" s="8">
@@ -1623,7 +1626,7 @@
   </sheetViews>
   <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
   <cols>
-    <col customWidth="1" min="1" max="1" width="20.75"/>
+    <col customWidth="1" min="1" max="1" width="25.63"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -1723,7 +1726,7 @@
       </c>
     </row>
     <row r="13">
-      <c r="A13" s="11" t="s">
+      <c r="A13" s="10" t="s">
         <v>13</v>
       </c>
       <c r="B13" s="8">
@@ -1734,7 +1737,7 @@
       <c r="A14" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="B14" s="19">
+      <c r="B14" s="20">
         <v>0.0</v>
       </c>
     </row>
@@ -1771,7 +1774,7 @@
       </c>
     </row>
     <row r="19">
-      <c r="A19" s="14" t="s">
+      <c r="A19" s="15" t="s">
         <v>19</v>
       </c>
       <c r="B19" s="8">
@@ -1779,7 +1782,7 @@
       </c>
     </row>
     <row r="20">
-      <c r="A20" s="14" t="s">
+      <c r="A20" s="15" t="s">
         <v>20</v>
       </c>
       <c r="B20" s="8">
@@ -1795,7 +1798,7 @@
       </c>
     </row>
     <row r="22">
-      <c r="A22" s="15" t="s">
+      <c r="A22" s="16" t="s">
         <v>22</v>
       </c>
       <c r="B22" s="6">
@@ -1803,7 +1806,7 @@
       </c>
     </row>
     <row r="23">
-      <c r="A23" s="16" t="s">
+      <c r="A23" s="17" t="s">
         <v>23</v>
       </c>
       <c r="B23" s="6">
@@ -1827,7 +1830,7 @@
       </c>
     </row>
     <row r="26">
-      <c r="A26" s="17" t="s">
+      <c r="A26" s="18" t="s">
         <v>26</v>
       </c>
       <c r="B26" s="8">
@@ -1835,7 +1838,7 @@
       </c>
     </row>
     <row r="27">
-      <c r="A27" s="17" t="s">
+      <c r="A27" s="19" t="s">
         <v>27</v>
       </c>
       <c r="B27" s="8">
@@ -1843,7 +1846,7 @@
       </c>
     </row>
     <row r="28">
-      <c r="A28" s="17" t="s">
+      <c r="A28" s="19" t="s">
         <v>28</v>
       </c>
       <c r="B28" s="8">
@@ -1873,7 +1876,7 @@
   </sheetViews>
   <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
   <cols>
-    <col customWidth="1" min="1" max="1" width="20.75"/>
+    <col customWidth="1" min="1" max="1" width="25.63"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -1973,7 +1976,7 @@
       </c>
     </row>
     <row r="13">
-      <c r="A13" s="11" t="s">
+      <c r="A13" s="10" t="s">
         <v>13</v>
       </c>
       <c r="B13" s="8">
@@ -1992,7 +1995,7 @@
       <c r="A15" s="12" t="s">
         <v>15</v>
       </c>
-      <c r="B15" s="19">
+      <c r="B15" s="20">
         <v>0.0</v>
       </c>
     </row>
@@ -2021,7 +2024,7 @@
       </c>
     </row>
     <row r="19">
-      <c r="A19" s="14" t="s">
+      <c r="A19" s="15" t="s">
         <v>19</v>
       </c>
       <c r="B19" s="8">
@@ -2029,7 +2032,7 @@
       </c>
     </row>
     <row r="20">
-      <c r="A20" s="14" t="s">
+      <c r="A20" s="15" t="s">
         <v>20</v>
       </c>
       <c r="B20" s="8">
@@ -2045,7 +2048,7 @@
       </c>
     </row>
     <row r="22">
-      <c r="A22" s="15" t="s">
+      <c r="A22" s="16" t="s">
         <v>22</v>
       </c>
       <c r="B22" s="6">
@@ -2053,7 +2056,7 @@
       </c>
     </row>
     <row r="23">
-      <c r="A23" s="16" t="s">
+      <c r="A23" s="17" t="s">
         <v>23</v>
       </c>
       <c r="B23" s="6">
@@ -2077,7 +2080,7 @@
       </c>
     </row>
     <row r="26">
-      <c r="A26" s="17" t="s">
+      <c r="A26" s="18" t="s">
         <v>26</v>
       </c>
       <c r="B26" s="8">
@@ -2085,7 +2088,7 @@
       </c>
     </row>
     <row r="27">
-      <c r="A27" s="17" t="s">
+      <c r="A27" s="19" t="s">
         <v>27</v>
       </c>
       <c r="B27" s="8">
@@ -2093,7 +2096,7 @@
       </c>
     </row>
     <row r="28">
-      <c r="A28" s="17" t="s">
+      <c r="A28" s="19" t="s">
         <v>28</v>
       </c>
       <c r="B28" s="8">
@@ -2123,7 +2126,7 @@
   </sheetViews>
   <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
   <cols>
-    <col customWidth="1" min="1" max="1" width="20.75"/>
+    <col customWidth="1" min="1" max="1" width="25.63"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -2223,7 +2226,7 @@
       </c>
     </row>
     <row r="13">
-      <c r="A13" s="11" t="s">
+      <c r="A13" s="10" t="s">
         <v>13</v>
       </c>
       <c r="B13" s="8">
@@ -2250,7 +2253,7 @@
       <c r="A16" s="13" t="s">
         <v>16</v>
       </c>
-      <c r="B16" s="19">
+      <c r="B16" s="20">
         <v>0.0</v>
       </c>
     </row>
@@ -2271,7 +2274,7 @@
       </c>
     </row>
     <row r="19">
-      <c r="A19" s="14" t="s">
+      <c r="A19" s="15" t="s">
         <v>19</v>
       </c>
       <c r="B19" s="8">
@@ -2279,7 +2282,7 @@
       </c>
     </row>
     <row r="20">
-      <c r="A20" s="14" t="s">
+      <c r="A20" s="15" t="s">
         <v>20</v>
       </c>
       <c r="B20" s="8">
@@ -2295,7 +2298,7 @@
       </c>
     </row>
     <row r="22">
-      <c r="A22" s="15" t="s">
+      <c r="A22" s="16" t="s">
         <v>22</v>
       </c>
       <c r="B22" s="6">
@@ -2303,7 +2306,7 @@
       </c>
     </row>
     <row r="23">
-      <c r="A23" s="16" t="s">
+      <c r="A23" s="17" t="s">
         <v>23</v>
       </c>
       <c r="B23" s="6">
@@ -2327,7 +2330,7 @@
       </c>
     </row>
     <row r="26">
-      <c r="A26" s="17" t="s">
+      <c r="A26" s="18" t="s">
         <v>26</v>
       </c>
       <c r="B26" s="8">
@@ -2335,7 +2338,7 @@
       </c>
     </row>
     <row r="27">
-      <c r="A27" s="17" t="s">
+      <c r="A27" s="19" t="s">
         <v>27</v>
       </c>
       <c r="B27" s="8">
@@ -2343,7 +2346,7 @@
       </c>
     </row>
     <row r="28">
-      <c r="A28" s="17" t="s">
+      <c r="A28" s="19" t="s">
         <v>28</v>
       </c>
       <c r="B28" s="8">
@@ -2373,7 +2376,7 @@
   </sheetViews>
   <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
   <cols>
-    <col customWidth="1" min="1" max="1" width="20.75"/>
+    <col customWidth="1" min="1" max="1" width="25.63"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -2473,7 +2476,7 @@
       </c>
     </row>
     <row r="13">
-      <c r="A13" s="11" t="s">
+      <c r="A13" s="10" t="s">
         <v>13</v>
       </c>
       <c r="B13" s="8">
@@ -2508,7 +2511,7 @@
       <c r="A17" s="12" t="s">
         <v>17</v>
       </c>
-      <c r="B17" s="19">
+      <c r="B17" s="20">
         <v>0.0</v>
       </c>
     </row>
@@ -2521,7 +2524,7 @@
       </c>
     </row>
     <row r="19">
-      <c r="A19" s="14" t="s">
+      <c r="A19" s="15" t="s">
         <v>19</v>
       </c>
       <c r="B19" s="8">
@@ -2529,7 +2532,7 @@
       </c>
     </row>
     <row r="20">
-      <c r="A20" s="14" t="s">
+      <c r="A20" s="15" t="s">
         <v>20</v>
       </c>
       <c r="B20" s="8">
@@ -2545,7 +2548,7 @@
       </c>
     </row>
     <row r="22">
-      <c r="A22" s="15" t="s">
+      <c r="A22" s="16" t="s">
         <v>22</v>
       </c>
       <c r="B22" s="6">
@@ -2553,7 +2556,7 @@
       </c>
     </row>
     <row r="23">
-      <c r="A23" s="16" t="s">
+      <c r="A23" s="17" t="s">
         <v>23</v>
       </c>
       <c r="B23" s="6">
@@ -2577,7 +2580,7 @@
       </c>
     </row>
     <row r="26">
-      <c r="A26" s="17" t="s">
+      <c r="A26" s="18" t="s">
         <v>26</v>
       </c>
       <c r="B26" s="8">
@@ -2585,7 +2588,7 @@
       </c>
     </row>
     <row r="27">
-      <c r="A27" s="17" t="s">
+      <c r="A27" s="19" t="s">
         <v>27</v>
       </c>
       <c r="B27" s="8">
@@ -2593,7 +2596,7 @@
       </c>
     </row>
     <row r="28">
-      <c r="A28" s="17" t="s">
+      <c r="A28" s="19" t="s">
         <v>28</v>
       </c>
       <c r="B28" s="8">
@@ -2623,7 +2626,7 @@
   </sheetViews>
   <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
   <cols>
-    <col customWidth="1" min="1" max="1" width="20.75"/>
+    <col customWidth="1" min="1" max="1" width="25.63"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -2723,7 +2726,7 @@
       </c>
     </row>
     <row r="13">
-      <c r="A13" s="11" t="s">
+      <c r="A13" s="10" t="s">
         <v>13</v>
       </c>
       <c r="B13" s="8">
@@ -2766,12 +2769,12 @@
       <c r="A18" s="14" t="s">
         <v>18</v>
       </c>
-      <c r="B18" s="19">
+      <c r="B18" s="20">
         <v>0.0</v>
       </c>
     </row>
     <row r="19">
-      <c r="A19" s="14" t="s">
+      <c r="A19" s="15" t="s">
         <v>19</v>
       </c>
       <c r="B19" s="8">
@@ -2779,7 +2782,7 @@
       </c>
     </row>
     <row r="20">
-      <c r="A20" s="14" t="s">
+      <c r="A20" s="15" t="s">
         <v>20</v>
       </c>
       <c r="B20" s="8">
@@ -2795,7 +2798,7 @@
       </c>
     </row>
     <row r="22">
-      <c r="A22" s="15" t="s">
+      <c r="A22" s="16" t="s">
         <v>22</v>
       </c>
       <c r="B22" s="6">
@@ -2803,7 +2806,7 @@
       </c>
     </row>
     <row r="23">
-      <c r="A23" s="16" t="s">
+      <c r="A23" s="17" t="s">
         <v>23</v>
       </c>
       <c r="B23" s="6">
@@ -2827,7 +2830,7 @@
       </c>
     </row>
     <row r="26">
-      <c r="A26" s="17" t="s">
+      <c r="A26" s="18" t="s">
         <v>26</v>
       </c>
       <c r="B26" s="8">
@@ -2835,7 +2838,7 @@
       </c>
     </row>
     <row r="27">
-      <c r="A27" s="17" t="s">
+      <c r="A27" s="19" t="s">
         <v>27</v>
       </c>
       <c r="B27" s="8">
@@ -2843,7 +2846,7 @@
       </c>
     </row>
     <row r="28">
-      <c r="A28" s="17" t="s">
+      <c r="A28" s="19" t="s">
         <v>28</v>
       </c>
       <c r="B28" s="8">
@@ -2873,7 +2876,7 @@
   </sheetViews>
   <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
   <cols>
-    <col customWidth="1" min="1" max="1" width="20.75"/>
+    <col customWidth="1" min="1" max="1" width="25.63"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -2973,7 +2976,7 @@
       </c>
     </row>
     <row r="13">
-      <c r="A13" s="11" t="s">
+      <c r="A13" s="10" t="s">
         <v>13</v>
       </c>
       <c r="B13" s="8">
@@ -3021,15 +3024,15 @@
       </c>
     </row>
     <row r="19">
-      <c r="A19" s="14" t="s">
+      <c r="A19" s="15" t="s">
         <v>19</v>
       </c>
-      <c r="B19" s="19">
+      <c r="B19" s="20">
         <v>0.0</v>
       </c>
     </row>
     <row r="20">
-      <c r="A20" s="14" t="s">
+      <c r="A20" s="15" t="s">
         <v>20</v>
       </c>
       <c r="B20" s="8">
@@ -3045,7 +3048,7 @@
       </c>
     </row>
     <row r="22">
-      <c r="A22" s="15" t="s">
+      <c r="A22" s="16" t="s">
         <v>22</v>
       </c>
       <c r="B22" s="6">
@@ -3053,7 +3056,7 @@
       </c>
     </row>
     <row r="23">
-      <c r="A23" s="16" t="s">
+      <c r="A23" s="17" t="s">
         <v>23</v>
       </c>
       <c r="B23" s="6">
@@ -3077,7 +3080,7 @@
       </c>
     </row>
     <row r="26">
-      <c r="A26" s="17" t="s">
+      <c r="A26" s="18" t="s">
         <v>26</v>
       </c>
       <c r="B26" s="8">
@@ -3085,7 +3088,7 @@
       </c>
     </row>
     <row r="27">
-      <c r="A27" s="17" t="s">
+      <c r="A27" s="19" t="s">
         <v>27</v>
       </c>
       <c r="B27" s="8">
@@ -3093,7 +3096,7 @@
       </c>
     </row>
     <row r="28">
-      <c r="A28" s="17" t="s">
+      <c r="A28" s="19" t="s">
         <v>28</v>
       </c>
       <c r="B28" s="8">
@@ -3123,7 +3126,7 @@
   </sheetViews>
   <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
   <cols>
-    <col customWidth="1" min="1" max="1" width="20.75"/>
+    <col customWidth="1" min="1" max="1" width="25.63"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -3223,7 +3226,7 @@
       </c>
     </row>
     <row r="13">
-      <c r="A13" s="11" t="s">
+      <c r="A13" s="10" t="s">
         <v>13</v>
       </c>
       <c r="B13" s="8">
@@ -3271,7 +3274,7 @@
       </c>
     </row>
     <row r="19">
-      <c r="A19" s="14" t="s">
+      <c r="A19" s="15" t="s">
         <v>19</v>
       </c>
       <c r="B19" s="8">
@@ -3279,10 +3282,10 @@
       </c>
     </row>
     <row r="20">
-      <c r="A20" s="14" t="s">
+      <c r="A20" s="15" t="s">
         <v>20</v>
       </c>
-      <c r="B20" s="19">
+      <c r="B20" s="20">
         <v>0.0</v>
       </c>
     </row>
@@ -3295,7 +3298,7 @@
       </c>
     </row>
     <row r="22">
-      <c r="A22" s="15" t="s">
+      <c r="A22" s="16" t="s">
         <v>22</v>
       </c>
       <c r="B22" s="6">
@@ -3303,7 +3306,7 @@
       </c>
     </row>
     <row r="23">
-      <c r="A23" s="16" t="s">
+      <c r="A23" s="17" t="s">
         <v>23</v>
       </c>
       <c r="B23" s="6">
@@ -3327,7 +3330,7 @@
       </c>
     </row>
     <row r="26">
-      <c r="A26" s="17" t="s">
+      <c r="A26" s="18" t="s">
         <v>26</v>
       </c>
       <c r="B26" s="8">
@@ -3335,7 +3338,7 @@
       </c>
     </row>
     <row r="27">
-      <c r="A27" s="17" t="s">
+      <c r="A27" s="19" t="s">
         <v>27</v>
       </c>
       <c r="B27" s="8">
@@ -3343,7 +3346,7 @@
       </c>
     </row>
     <row r="28">
-      <c r="A28" s="17" t="s">
+      <c r="A28" s="19" t="s">
         <v>28</v>
       </c>
       <c r="B28" s="8">
@@ -3373,7 +3376,7 @@
   </sheetViews>
   <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
   <cols>
-    <col customWidth="1" min="1" max="1" width="20.75"/>
+    <col customWidth="1" min="1" max="1" width="25.63"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -3473,7 +3476,7 @@
       </c>
     </row>
     <row r="13">
-      <c r="A13" s="11" t="s">
+      <c r="A13" s="10" t="s">
         <v>13</v>
       </c>
       <c r="B13" s="8">
@@ -3521,7 +3524,7 @@
       </c>
     </row>
     <row r="19">
-      <c r="A19" s="14" t="s">
+      <c r="A19" s="15" t="s">
         <v>19</v>
       </c>
       <c r="B19" s="8">
@@ -3529,7 +3532,7 @@
       </c>
     </row>
     <row r="20">
-      <c r="A20" s="14" t="s">
+      <c r="A20" s="15" t="s">
         <v>20</v>
       </c>
       <c r="B20" s="8">
@@ -3545,7 +3548,7 @@
       </c>
     </row>
     <row r="22">
-      <c r="A22" s="15" t="s">
+      <c r="A22" s="16" t="s">
         <v>22</v>
       </c>
       <c r="B22" s="6">
@@ -3553,7 +3556,7 @@
       </c>
     </row>
     <row r="23">
-      <c r="A23" s="16" t="s">
+      <c r="A23" s="17" t="s">
         <v>23</v>
       </c>
       <c r="B23" s="6">
@@ -3577,7 +3580,7 @@
       </c>
     </row>
     <row r="26">
-      <c r="A26" s="17" t="s">
+      <c r="A26" s="18" t="s">
         <v>26</v>
       </c>
       <c r="B26" s="8">
@@ -3585,7 +3588,7 @@
       </c>
     </row>
     <row r="27">
-      <c r="A27" s="17" t="s">
+      <c r="A27" s="19" t="s">
         <v>27</v>
       </c>
       <c r="B27" s="8">
@@ -3593,7 +3596,7 @@
       </c>
     </row>
     <row r="28">
-      <c r="A28" s="17" t="s">
+      <c r="A28" s="19" t="s">
         <v>28</v>
       </c>
       <c r="B28" s="8">
@@ -3623,7 +3626,7 @@
   </sheetViews>
   <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
   <cols>
-    <col customWidth="1" min="1" max="1" width="20.75"/>
+    <col customWidth="1" min="1" max="1" width="25.63"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -3723,7 +3726,7 @@
       </c>
     </row>
     <row r="13">
-      <c r="A13" s="11" t="s">
+      <c r="A13" s="10" t="s">
         <v>13</v>
       </c>
       <c r="B13" s="8">
@@ -3771,7 +3774,7 @@
       </c>
     </row>
     <row r="19">
-      <c r="A19" s="14" t="s">
+      <c r="A19" s="15" t="s">
         <v>19</v>
       </c>
       <c r="B19" s="8">
@@ -3779,7 +3782,7 @@
       </c>
     </row>
     <row r="20">
-      <c r="A20" s="14" t="s">
+      <c r="A20" s="15" t="s">
         <v>20</v>
       </c>
       <c r="B20" s="8">
@@ -3790,12 +3793,12 @@
       <c r="A21" s="14" t="s">
         <v>21</v>
       </c>
-      <c r="B21" s="19">
+      <c r="B21" s="20">
         <v>0.0</v>
       </c>
     </row>
     <row r="22">
-      <c r="A22" s="15" t="s">
+      <c r="A22" s="16" t="s">
         <v>22</v>
       </c>
       <c r="B22" s="6">
@@ -3803,7 +3806,7 @@
       </c>
     </row>
     <row r="23">
-      <c r="A23" s="16" t="s">
+      <c r="A23" s="17" t="s">
         <v>23</v>
       </c>
       <c r="B23" s="6">
@@ -3827,7 +3830,7 @@
       </c>
     </row>
     <row r="26">
-      <c r="A26" s="17" t="s">
+      <c r="A26" s="18" t="s">
         <v>26</v>
       </c>
       <c r="B26" s="8">
@@ -3835,7 +3838,7 @@
       </c>
     </row>
     <row r="27">
-      <c r="A27" s="17" t="s">
+      <c r="A27" s="19" t="s">
         <v>27</v>
       </c>
       <c r="B27" s="8">
@@ -3843,7 +3846,7 @@
       </c>
     </row>
     <row r="28">
-      <c r="A28" s="17" t="s">
+      <c r="A28" s="19" t="s">
         <v>28</v>
       </c>
       <c r="B28" s="8">
@@ -3873,7 +3876,7 @@
   </sheetViews>
   <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
   <cols>
-    <col customWidth="1" min="1" max="1" width="20.75"/>
+    <col customWidth="1" min="1" max="1" width="25.63"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -3973,7 +3976,7 @@
       </c>
     </row>
     <row r="13">
-      <c r="A13" s="11" t="s">
+      <c r="A13" s="10" t="s">
         <v>13</v>
       </c>
       <c r="B13" s="8">
@@ -4021,7 +4024,7 @@
       </c>
     </row>
     <row r="19">
-      <c r="A19" s="14" t="s">
+      <c r="A19" s="15" t="s">
         <v>19</v>
       </c>
       <c r="B19" s="8">
@@ -4029,7 +4032,7 @@
       </c>
     </row>
     <row r="20">
-      <c r="A20" s="14" t="s">
+      <c r="A20" s="15" t="s">
         <v>20</v>
       </c>
       <c r="B20" s="8">
@@ -4045,7 +4048,7 @@
       </c>
     </row>
     <row r="22">
-      <c r="A22" s="15" t="s">
+      <c r="A22" s="16" t="s">
         <v>22</v>
       </c>
       <c r="B22" s="4">
@@ -4053,7 +4056,7 @@
       </c>
     </row>
     <row r="23">
-      <c r="A23" s="16" t="s">
+      <c r="A23" s="17" t="s">
         <v>23</v>
       </c>
       <c r="B23" s="6">
@@ -4077,7 +4080,7 @@
       </c>
     </row>
     <row r="26">
-      <c r="A26" s="17" t="s">
+      <c r="A26" s="18" t="s">
         <v>26</v>
       </c>
       <c r="B26" s="8">
@@ -4085,7 +4088,7 @@
       </c>
     </row>
     <row r="27">
-      <c r="A27" s="17" t="s">
+      <c r="A27" s="19" t="s">
         <v>27</v>
       </c>
       <c r="B27" s="8">
@@ -4093,7 +4096,7 @@
       </c>
     </row>
     <row r="28">
-      <c r="A28" s="17" t="s">
+      <c r="A28" s="19" t="s">
         <v>28</v>
       </c>
       <c r="B28" s="8">
@@ -4123,7 +4126,7 @@
   </sheetViews>
   <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
   <cols>
-    <col customWidth="1" min="1" max="1" width="20.75"/>
+    <col customWidth="1" min="1" max="1" width="25.63"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -4223,7 +4226,7 @@
       </c>
     </row>
     <row r="13">
-      <c r="A13" s="11" t="s">
+      <c r="A13" s="10" t="s">
         <v>13</v>
       </c>
       <c r="B13" s="8">
@@ -4271,7 +4274,7 @@
       </c>
     </row>
     <row r="19">
-      <c r="A19" s="14" t="s">
+      <c r="A19" s="15" t="s">
         <v>19</v>
       </c>
       <c r="B19" s="8">
@@ -4279,7 +4282,7 @@
       </c>
     </row>
     <row r="20">
-      <c r="A20" s="14" t="s">
+      <c r="A20" s="15" t="s">
         <v>20</v>
       </c>
       <c r="B20" s="8">
@@ -4295,7 +4298,7 @@
       </c>
     </row>
     <row r="22">
-      <c r="A22" s="15" t="s">
+      <c r="A22" s="16" t="s">
         <v>22</v>
       </c>
       <c r="B22" s="6">
@@ -4303,7 +4306,7 @@
       </c>
     </row>
     <row r="23">
-      <c r="A23" s="16" t="s">
+      <c r="A23" s="17" t="s">
         <v>23</v>
       </c>
       <c r="B23" s="4">
@@ -4327,7 +4330,7 @@
       </c>
     </row>
     <row r="26">
-      <c r="A26" s="17" t="s">
+      <c r="A26" s="18" t="s">
         <v>26</v>
       </c>
       <c r="B26" s="8">
@@ -4335,7 +4338,7 @@
       </c>
     </row>
     <row r="27">
-      <c r="A27" s="17" t="s">
+      <c r="A27" s="19" t="s">
         <v>27</v>
       </c>
       <c r="B27" s="8">
@@ -4343,7 +4346,7 @@
       </c>
     </row>
     <row r="28">
-      <c r="A28" s="17" t="s">
+      <c r="A28" s="19" t="s">
         <v>28</v>
       </c>
       <c r="B28" s="8">
@@ -4373,7 +4376,7 @@
   </sheetViews>
   <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
   <cols>
-    <col customWidth="1" min="1" max="1" width="20.75"/>
+    <col customWidth="1" min="1" max="1" width="25.63"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -4473,7 +4476,7 @@
       </c>
     </row>
     <row r="13">
-      <c r="A13" s="11" t="s">
+      <c r="A13" s="10" t="s">
         <v>13</v>
       </c>
       <c r="B13" s="8">
@@ -4521,7 +4524,7 @@
       </c>
     </row>
     <row r="19">
-      <c r="A19" s="14" t="s">
+      <c r="A19" s="15" t="s">
         <v>19</v>
       </c>
       <c r="B19" s="8">
@@ -4529,7 +4532,7 @@
       </c>
     </row>
     <row r="20">
-      <c r="A20" s="14" t="s">
+      <c r="A20" s="15" t="s">
         <v>20</v>
       </c>
       <c r="B20" s="8">
@@ -4545,7 +4548,7 @@
       </c>
     </row>
     <row r="22">
-      <c r="A22" s="15" t="s">
+      <c r="A22" s="16" t="s">
         <v>22</v>
       </c>
       <c r="B22" s="6">
@@ -4553,7 +4556,7 @@
       </c>
     </row>
     <row r="23">
-      <c r="A23" s="16" t="s">
+      <c r="A23" s="17" t="s">
         <v>23</v>
       </c>
       <c r="B23" s="6">
@@ -4577,7 +4580,7 @@
       </c>
     </row>
     <row r="26">
-      <c r="A26" s="17" t="s">
+      <c r="A26" s="18" t="s">
         <v>26</v>
       </c>
       <c r="B26" s="8">
@@ -4585,7 +4588,7 @@
       </c>
     </row>
     <row r="27">
-      <c r="A27" s="17" t="s">
+      <c r="A27" s="19" t="s">
         <v>27</v>
       </c>
       <c r="B27" s="8">
@@ -4593,7 +4596,7 @@
       </c>
     </row>
     <row r="28">
-      <c r="A28" s="17" t="s">
+      <c r="A28" s="19" t="s">
         <v>28</v>
       </c>
       <c r="B28" s="8">
@@ -4623,7 +4626,7 @@
   </sheetViews>
   <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
   <cols>
-    <col customWidth="1" min="1" max="1" width="20.75"/>
+    <col customWidth="1" min="1" max="1" width="25.63"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -4723,7 +4726,7 @@
       </c>
     </row>
     <row r="13">
-      <c r="A13" s="11" t="s">
+      <c r="A13" s="10" t="s">
         <v>13</v>
       </c>
       <c r="B13" s="8">
@@ -4771,7 +4774,7 @@
       </c>
     </row>
     <row r="19">
-      <c r="A19" s="14" t="s">
+      <c r="A19" s="15" t="s">
         <v>19</v>
       </c>
       <c r="B19" s="8">
@@ -4779,7 +4782,7 @@
       </c>
     </row>
     <row r="20">
-      <c r="A20" s="14" t="s">
+      <c r="A20" s="15" t="s">
         <v>20</v>
       </c>
       <c r="B20" s="8">
@@ -4795,7 +4798,7 @@
       </c>
     </row>
     <row r="22">
-      <c r="A22" s="15" t="s">
+      <c r="A22" s="16" t="s">
         <v>22</v>
       </c>
       <c r="B22" s="6">
@@ -4803,7 +4806,7 @@
       </c>
     </row>
     <row r="23">
-      <c r="A23" s="16" t="s">
+      <c r="A23" s="17" t="s">
         <v>23</v>
       </c>
       <c r="B23" s="6">
@@ -4827,7 +4830,7 @@
       </c>
     </row>
     <row r="26">
-      <c r="A26" s="17" t="s">
+      <c r="A26" s="18" t="s">
         <v>26</v>
       </c>
       <c r="B26" s="8">
@@ -4835,7 +4838,7 @@
       </c>
     </row>
     <row r="27">
-      <c r="A27" s="17" t="s">
+      <c r="A27" s="19" t="s">
         <v>27</v>
       </c>
       <c r="B27" s="8">
@@ -4843,7 +4846,7 @@
       </c>
     </row>
     <row r="28">
-      <c r="A28" s="17" t="s">
+      <c r="A28" s="19" t="s">
         <v>28</v>
       </c>
       <c r="B28" s="8">
@@ -4873,7 +4876,7 @@
   </sheetViews>
   <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
   <cols>
-    <col customWidth="1" min="1" max="1" width="20.75"/>
+    <col customWidth="1" min="1" max="1" width="25.63"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -4973,7 +4976,7 @@
       </c>
     </row>
     <row r="13">
-      <c r="A13" s="11" t="s">
+      <c r="A13" s="10" t="s">
         <v>13</v>
       </c>
       <c r="B13" s="8">
@@ -5021,7 +5024,7 @@
       </c>
     </row>
     <row r="19">
-      <c r="A19" s="14" t="s">
+      <c r="A19" s="15" t="s">
         <v>19</v>
       </c>
       <c r="B19" s="8">
@@ -5029,7 +5032,7 @@
       </c>
     </row>
     <row r="20">
-      <c r="A20" s="14" t="s">
+      <c r="A20" s="15" t="s">
         <v>20</v>
       </c>
       <c r="B20" s="8">
@@ -5045,7 +5048,7 @@
       </c>
     </row>
     <row r="22">
-      <c r="A22" s="15" t="s">
+      <c r="A22" s="16" t="s">
         <v>22</v>
       </c>
       <c r="B22" s="6">
@@ -5053,7 +5056,7 @@
       </c>
     </row>
     <row r="23">
-      <c r="A23" s="16" t="s">
+      <c r="A23" s="17" t="s">
         <v>23</v>
       </c>
       <c r="B23" s="6">
@@ -5077,15 +5080,15 @@
       </c>
     </row>
     <row r="26">
-      <c r="A26" s="17" t="s">
+      <c r="A26" s="18" t="s">
         <v>26</v>
       </c>
-      <c r="B26" s="19">
+      <c r="B26" s="20">
         <v>0.0</v>
       </c>
     </row>
     <row r="27">
-      <c r="A27" s="17" t="s">
+      <c r="A27" s="19" t="s">
         <v>27</v>
       </c>
       <c r="B27" s="8">
@@ -5093,7 +5096,7 @@
       </c>
     </row>
     <row r="28">
-      <c r="A28" s="17" t="s">
+      <c r="A28" s="19" t="s">
         <v>28</v>
       </c>
       <c r="B28" s="8">
@@ -5123,7 +5126,7 @@
   </sheetViews>
   <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
   <cols>
-    <col customWidth="1" min="1" max="1" width="20.75"/>
+    <col customWidth="1" min="1" max="1" width="25.63"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -5138,7 +5141,7 @@
       <c r="A2" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="20">
+      <c r="B2" s="21">
         <v>557.0</v>
       </c>
     </row>
@@ -5146,7 +5149,7 @@
       <c r="A3" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="20">
+      <c r="B3" s="21">
         <v>441.0</v>
       </c>
     </row>
@@ -5154,7 +5157,7 @@
       <c r="A4" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="B4" s="20">
+      <c r="B4" s="21">
         <v>418.0</v>
       </c>
     </row>
@@ -5162,7 +5165,7 @@
       <c r="A5" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="B5" s="20">
+      <c r="B5" s="21">
         <v>521.0</v>
       </c>
     </row>
@@ -5223,7 +5226,7 @@
       </c>
     </row>
     <row r="13">
-      <c r="A13" s="11" t="s">
+      <c r="A13" s="10" t="s">
         <v>13</v>
       </c>
       <c r="B13" s="8">
@@ -5271,7 +5274,7 @@
       </c>
     </row>
     <row r="19">
-      <c r="A19" s="14" t="s">
+      <c r="A19" s="15" t="s">
         <v>19</v>
       </c>
       <c r="B19" s="8">
@@ -5279,7 +5282,7 @@
       </c>
     </row>
     <row r="20">
-      <c r="A20" s="14" t="s">
+      <c r="A20" s="15" t="s">
         <v>20</v>
       </c>
       <c r="B20" s="8">
@@ -5295,7 +5298,7 @@
       </c>
     </row>
     <row r="22">
-      <c r="A22" s="15" t="s">
+      <c r="A22" s="16" t="s">
         <v>22</v>
       </c>
       <c r="B22" s="6">
@@ -5303,7 +5306,7 @@
       </c>
     </row>
     <row r="23">
-      <c r="A23" s="16" t="s">
+      <c r="A23" s="17" t="s">
         <v>23</v>
       </c>
       <c r="B23" s="6">
@@ -5327,7 +5330,7 @@
       </c>
     </row>
     <row r="26">
-      <c r="A26" s="17" t="s">
+      <c r="A26" s="18" t="s">
         <v>26</v>
       </c>
       <c r="B26" s="8">
@@ -5335,15 +5338,15 @@
       </c>
     </row>
     <row r="27">
-      <c r="A27" s="17" t="s">
+      <c r="A27" s="19" t="s">
         <v>27</v>
       </c>
-      <c r="B27" s="19">
+      <c r="B27" s="20">
         <v>0.0</v>
       </c>
     </row>
     <row r="28">
-      <c r="A28" s="17" t="s">
+      <c r="A28" s="19" t="s">
         <v>28</v>
       </c>
       <c r="B28" s="8">
@@ -5373,7 +5376,7 @@
   </sheetViews>
   <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
   <cols>
-    <col customWidth="1" min="1" max="1" width="20.75"/>
+    <col customWidth="1" min="1" max="1" width="25.63"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -5473,7 +5476,7 @@
       </c>
     </row>
     <row r="13">
-      <c r="A13" s="11" t="s">
+      <c r="A13" s="10" t="s">
         <v>13</v>
       </c>
       <c r="B13" s="8">
@@ -5521,7 +5524,7 @@
       </c>
     </row>
     <row r="19">
-      <c r="A19" s="14" t="s">
+      <c r="A19" s="15" t="s">
         <v>19</v>
       </c>
       <c r="B19" s="8">
@@ -5529,7 +5532,7 @@
       </c>
     </row>
     <row r="20">
-      <c r="A20" s="14" t="s">
+      <c r="A20" s="15" t="s">
         <v>20</v>
       </c>
       <c r="B20" s="8">
@@ -5545,7 +5548,7 @@
       </c>
     </row>
     <row r="22">
-      <c r="A22" s="15" t="s">
+      <c r="A22" s="16" t="s">
         <v>22</v>
       </c>
       <c r="B22" s="6">
@@ -5553,7 +5556,7 @@
       </c>
     </row>
     <row r="23">
-      <c r="A23" s="16" t="s">
+      <c r="A23" s="17" t="s">
         <v>23</v>
       </c>
       <c r="B23" s="6">
@@ -5577,7 +5580,7 @@
       </c>
     </row>
     <row r="26">
-      <c r="A26" s="17" t="s">
+      <c r="A26" s="18" t="s">
         <v>26</v>
       </c>
       <c r="B26" s="8">
@@ -5585,7 +5588,7 @@
       </c>
     </row>
     <row r="27">
-      <c r="A27" s="17" t="s">
+      <c r="A27" s="19" t="s">
         <v>27</v>
       </c>
       <c r="B27" s="8">
@@ -5593,10 +5596,10 @@
       </c>
     </row>
     <row r="28">
-      <c r="A28" s="17" t="s">
+      <c r="A28" s="19" t="s">
         <v>28</v>
       </c>
-      <c r="B28" s="19">
+      <c r="B28" s="20">
         <v>0.0</v>
       </c>
     </row>
@@ -5623,7 +5626,7 @@
   </sheetViews>
   <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
   <cols>
-    <col customWidth="1" min="1" max="1" width="20.75"/>
+    <col customWidth="1" min="1" max="1" width="25.63"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -5723,7 +5726,7 @@
       </c>
     </row>
     <row r="13">
-      <c r="A13" s="11" t="s">
+      <c r="A13" s="10" t="s">
         <v>13</v>
       </c>
       <c r="B13" s="8">
@@ -5771,7 +5774,7 @@
       </c>
     </row>
     <row r="19">
-      <c r="A19" s="14" t="s">
+      <c r="A19" s="15" t="s">
         <v>19</v>
       </c>
       <c r="B19" s="8">
@@ -5779,7 +5782,7 @@
       </c>
     </row>
     <row r="20">
-      <c r="A20" s="14" t="s">
+      <c r="A20" s="15" t="s">
         <v>20</v>
       </c>
       <c r="B20" s="8">
@@ -5795,7 +5798,7 @@
       </c>
     </row>
     <row r="22">
-      <c r="A22" s="15" t="s">
+      <c r="A22" s="16" t="s">
         <v>22</v>
       </c>
       <c r="B22" s="6">
@@ -5803,7 +5806,7 @@
       </c>
     </row>
     <row r="23">
-      <c r="A23" s="16" t="s">
+      <c r="A23" s="17" t="s">
         <v>23</v>
       </c>
       <c r="B23" s="6">
@@ -5827,7 +5830,7 @@
       </c>
     </row>
     <row r="26">
-      <c r="A26" s="17" t="s">
+      <c r="A26" s="18" t="s">
         <v>26</v>
       </c>
       <c r="B26" s="8">
@@ -5835,7 +5838,7 @@
       </c>
     </row>
     <row r="27">
-      <c r="A27" s="17" t="s">
+      <c r="A27" s="19" t="s">
         <v>27</v>
       </c>
       <c r="B27" s="8">
@@ -5843,7 +5846,7 @@
       </c>
     </row>
     <row r="28">
-      <c r="A28" s="17" t="s">
+      <c r="A28" s="19" t="s">
         <v>28</v>
       </c>
       <c r="B28" s="8">
@@ -5854,7 +5857,7 @@
       <c r="A29" s="18" t="s">
         <v>29</v>
       </c>
-      <c r="B29" s="19">
+      <c r="B29" s="20">
         <v>0.0</v>
       </c>
     </row>
@@ -5873,7 +5876,7 @@
   </sheetViews>
   <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
   <cols>
-    <col customWidth="1" min="1" max="1" width="20.75"/>
+    <col customWidth="1" min="1" max="1" width="25.63"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -5973,7 +5976,7 @@
       </c>
     </row>
     <row r="13">
-      <c r="A13" s="11" t="s">
+      <c r="A13" s="10" t="s">
         <v>13</v>
       </c>
       <c r="B13" s="8">
@@ -6021,7 +6024,7 @@
       </c>
     </row>
     <row r="19">
-      <c r="A19" s="14" t="s">
+      <c r="A19" s="15" t="s">
         <v>19</v>
       </c>
       <c r="B19" s="8">
@@ -6029,7 +6032,7 @@
       </c>
     </row>
     <row r="20">
-      <c r="A20" s="14" t="s">
+      <c r="A20" s="15" t="s">
         <v>20</v>
       </c>
       <c r="B20" s="8">
@@ -6045,7 +6048,7 @@
       </c>
     </row>
     <row r="22">
-      <c r="A22" s="15" t="s">
+      <c r="A22" s="16" t="s">
         <v>22</v>
       </c>
       <c r="B22" s="6">
@@ -6053,7 +6056,7 @@
       </c>
     </row>
     <row r="23">
-      <c r="A23" s="16" t="s">
+      <c r="A23" s="17" t="s">
         <v>23</v>
       </c>
       <c r="B23" s="6">
@@ -6077,7 +6080,7 @@
       </c>
     </row>
     <row r="26">
-      <c r="A26" s="17" t="s">
+      <c r="A26" s="18" t="s">
         <v>26</v>
       </c>
       <c r="B26" s="8">
@@ -6085,7 +6088,7 @@
       </c>
     </row>
     <row r="27">
-      <c r="A27" s="17" t="s">
+      <c r="A27" s="19" t="s">
         <v>27</v>
       </c>
       <c r="B27" s="8">
@@ -6093,7 +6096,7 @@
       </c>
     </row>
     <row r="28">
-      <c r="A28" s="17" t="s">
+      <c r="A28" s="19" t="s">
         <v>28</v>
       </c>
       <c r="B28" s="8">
@@ -6123,7 +6126,7 @@
   </sheetViews>
   <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
   <cols>
-    <col customWidth="1" min="1" max="1" width="20.75"/>
+    <col customWidth="1" min="1" max="1" width="25.63"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -6223,7 +6226,7 @@
       </c>
     </row>
     <row r="13">
-      <c r="A13" s="11" t="s">
+      <c r="A13" s="10" t="s">
         <v>13</v>
       </c>
       <c r="B13" s="8">
@@ -6271,7 +6274,7 @@
       </c>
     </row>
     <row r="19">
-      <c r="A19" s="14" t="s">
+      <c r="A19" s="15" t="s">
         <v>19</v>
       </c>
       <c r="B19" s="8">
@@ -6279,7 +6282,7 @@
       </c>
     </row>
     <row r="20">
-      <c r="A20" s="14" t="s">
+      <c r="A20" s="15" t="s">
         <v>20</v>
       </c>
       <c r="B20" s="8">
@@ -6295,7 +6298,7 @@
       </c>
     </row>
     <row r="22">
-      <c r="A22" s="15" t="s">
+      <c r="A22" s="16" t="s">
         <v>22</v>
       </c>
       <c r="B22" s="6">
@@ -6303,7 +6306,7 @@
       </c>
     </row>
     <row r="23">
-      <c r="A23" s="16" t="s">
+      <c r="A23" s="17" t="s">
         <v>23</v>
       </c>
       <c r="B23" s="6">
@@ -6327,7 +6330,7 @@
       </c>
     </row>
     <row r="26">
-      <c r="A26" s="17" t="s">
+      <c r="A26" s="18" t="s">
         <v>26</v>
       </c>
       <c r="B26" s="8">
@@ -6335,7 +6338,7 @@
       </c>
     </row>
     <row r="27">
-      <c r="A27" s="17" t="s">
+      <c r="A27" s="19" t="s">
         <v>27</v>
       </c>
       <c r="B27" s="8">
@@ -6343,7 +6346,7 @@
       </c>
     </row>
     <row r="28">
-      <c r="A28" s="17" t="s">
+      <c r="A28" s="19" t="s">
         <v>28</v>
       </c>
       <c r="B28" s="8">
@@ -6373,7 +6376,7 @@
   </sheetViews>
   <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
   <cols>
-    <col customWidth="1" min="1" max="1" width="20.75"/>
+    <col customWidth="1" min="1" max="1" width="25.63"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -6420,7 +6423,7 @@
       <c r="A6" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="B6" s="19">
+      <c r="B6" s="20">
         <v>0.0</v>
       </c>
     </row>
@@ -6473,7 +6476,7 @@
       </c>
     </row>
     <row r="13">
-      <c r="A13" s="11" t="s">
+      <c r="A13" s="10" t="s">
         <v>13</v>
       </c>
       <c r="B13" s="8">
@@ -6521,7 +6524,7 @@
       </c>
     </row>
     <row r="19">
-      <c r="A19" s="14" t="s">
+      <c r="A19" s="15" t="s">
         <v>19</v>
       </c>
       <c r="B19" s="8">
@@ -6529,7 +6532,7 @@
       </c>
     </row>
     <row r="20">
-      <c r="A20" s="14" t="s">
+      <c r="A20" s="15" t="s">
         <v>20</v>
       </c>
       <c r="B20" s="8">
@@ -6545,7 +6548,7 @@
       </c>
     </row>
     <row r="22">
-      <c r="A22" s="15" t="s">
+      <c r="A22" s="16" t="s">
         <v>22</v>
       </c>
       <c r="B22" s="6">
@@ -6553,7 +6556,7 @@
       </c>
     </row>
     <row r="23">
-      <c r="A23" s="16" t="s">
+      <c r="A23" s="17" t="s">
         <v>23</v>
       </c>
       <c r="B23" s="6">
@@ -6577,7 +6580,7 @@
       </c>
     </row>
     <row r="26">
-      <c r="A26" s="17" t="s">
+      <c r="A26" s="18" t="s">
         <v>26</v>
       </c>
       <c r="B26" s="8">
@@ -6585,7 +6588,7 @@
       </c>
     </row>
     <row r="27">
-      <c r="A27" s="17" t="s">
+      <c r="A27" s="19" t="s">
         <v>27</v>
       </c>
       <c r="B27" s="8">
@@ -6593,7 +6596,7 @@
       </c>
     </row>
     <row r="28">
-      <c r="A28" s="17" t="s">
+      <c r="A28" s="19" t="s">
         <v>28</v>
       </c>
       <c r="B28" s="8">
@@ -6623,7 +6626,7 @@
   </sheetViews>
   <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
   <cols>
-    <col customWidth="1" min="1" max="1" width="20.75"/>
+    <col customWidth="1" min="1" max="1" width="25.63"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -6678,7 +6681,7 @@
       <c r="A7" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="B7" s="19">
+      <c r="B7" s="20">
         <v>0.0</v>
       </c>
     </row>
@@ -6723,7 +6726,7 @@
       </c>
     </row>
     <row r="13">
-      <c r="A13" s="11" t="s">
+      <c r="A13" s="10" t="s">
         <v>13</v>
       </c>
       <c r="B13" s="8">
@@ -6771,7 +6774,7 @@
       </c>
     </row>
     <row r="19">
-      <c r="A19" s="14" t="s">
+      <c r="A19" s="15" t="s">
         <v>19</v>
       </c>
       <c r="B19" s="8">
@@ -6779,7 +6782,7 @@
       </c>
     </row>
     <row r="20">
-      <c r="A20" s="14" t="s">
+      <c r="A20" s="15" t="s">
         <v>20</v>
       </c>
       <c r="B20" s="8">
@@ -6795,7 +6798,7 @@
       </c>
     </row>
     <row r="22">
-      <c r="A22" s="15" t="s">
+      <c r="A22" s="16" t="s">
         <v>22</v>
       </c>
       <c r="B22" s="6">
@@ -6803,7 +6806,7 @@
       </c>
     </row>
     <row r="23">
-      <c r="A23" s="16" t="s">
+      <c r="A23" s="17" t="s">
         <v>23</v>
       </c>
       <c r="B23" s="6">
@@ -6827,7 +6830,7 @@
       </c>
     </row>
     <row r="26">
-      <c r="A26" s="17" t="s">
+      <c r="A26" s="18" t="s">
         <v>26</v>
       </c>
       <c r="B26" s="8">
@@ -6835,7 +6838,7 @@
       </c>
     </row>
     <row r="27">
-      <c r="A27" s="17" t="s">
+      <c r="A27" s="19" t="s">
         <v>27</v>
       </c>
       <c r="B27" s="8">
@@ -6843,7 +6846,7 @@
       </c>
     </row>
     <row r="28">
-      <c r="A28" s="17" t="s">
+      <c r="A28" s="19" t="s">
         <v>28</v>
       </c>
       <c r="B28" s="8">
@@ -6873,7 +6876,7 @@
   </sheetViews>
   <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
   <cols>
-    <col customWidth="1" min="1" max="1" width="20.75"/>
+    <col customWidth="1" min="1" max="1" width="25.63"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -6936,7 +6939,7 @@
       <c r="A8" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="B8" s="19">
+      <c r="B8" s="20">
         <v>0.0</v>
       </c>
     </row>
@@ -6973,7 +6976,7 @@
       </c>
     </row>
     <row r="13">
-      <c r="A13" s="11" t="s">
+      <c r="A13" s="10" t="s">
         <v>13</v>
       </c>
       <c r="B13" s="8">
@@ -7021,7 +7024,7 @@
       </c>
     </row>
     <row r="19">
-      <c r="A19" s="14" t="s">
+      <c r="A19" s="15" t="s">
         <v>19</v>
       </c>
       <c r="B19" s="8">
@@ -7029,7 +7032,7 @@
       </c>
     </row>
     <row r="20">
-      <c r="A20" s="14" t="s">
+      <c r="A20" s="15" t="s">
         <v>20</v>
       </c>
       <c r="B20" s="8">
@@ -7045,7 +7048,7 @@
       </c>
     </row>
     <row r="22">
-      <c r="A22" s="15" t="s">
+      <c r="A22" s="16" t="s">
         <v>22</v>
       </c>
       <c r="B22" s="6">
@@ -7053,7 +7056,7 @@
       </c>
     </row>
     <row r="23">
-      <c r="A23" s="16" t="s">
+      <c r="A23" s="17" t="s">
         <v>23</v>
       </c>
       <c r="B23" s="6">
@@ -7077,7 +7080,7 @@
       </c>
     </row>
     <row r="26">
-      <c r="A26" s="17" t="s">
+      <c r="A26" s="18" t="s">
         <v>26</v>
       </c>
       <c r="B26" s="8">
@@ -7085,7 +7088,7 @@
       </c>
     </row>
     <row r="27">
-      <c r="A27" s="17" t="s">
+      <c r="A27" s="19" t="s">
         <v>27</v>
       </c>
       <c r="B27" s="8">
@@ -7093,7 +7096,7 @@
       </c>
     </row>
     <row r="28">
-      <c r="A28" s="17" t="s">
+      <c r="A28" s="19" t="s">
         <v>28</v>
       </c>
       <c r="B28" s="8">
@@ -7123,7 +7126,7 @@
   </sheetViews>
   <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
   <cols>
-    <col customWidth="1" min="1" max="1" width="20.75"/>
+    <col customWidth="1" min="1" max="1" width="25.63"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -7194,7 +7197,7 @@
       <c r="A9" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="B9" s="19">
+      <c r="B9" s="20">
         <v>0.0</v>
       </c>
     </row>
@@ -7223,7 +7226,7 @@
       </c>
     </row>
     <row r="13">
-      <c r="A13" s="11" t="s">
+      <c r="A13" s="10" t="s">
         <v>13</v>
       </c>
       <c r="B13" s="8">
@@ -7271,7 +7274,7 @@
       </c>
     </row>
     <row r="19">
-      <c r="A19" s="14" t="s">
+      <c r="A19" s="15" t="s">
         <v>19</v>
       </c>
       <c r="B19" s="8">
@@ -7279,7 +7282,7 @@
       </c>
     </row>
     <row r="20">
-      <c r="A20" s="14" t="s">
+      <c r="A20" s="15" t="s">
         <v>20</v>
       </c>
       <c r="B20" s="8">
@@ -7295,7 +7298,7 @@
       </c>
     </row>
     <row r="22">
-      <c r="A22" s="15" t="s">
+      <c r="A22" s="16" t="s">
         <v>22</v>
       </c>
       <c r="B22" s="6">
@@ -7303,7 +7306,7 @@
       </c>
     </row>
     <row r="23">
-      <c r="A23" s="16" t="s">
+      <c r="A23" s="17" t="s">
         <v>23</v>
       </c>
       <c r="B23" s="6">
@@ -7327,7 +7330,7 @@
       </c>
     </row>
     <row r="26">
-      <c r="A26" s="17" t="s">
+      <c r="A26" s="18" t="s">
         <v>26</v>
       </c>
       <c r="B26" s="8">
@@ -7335,7 +7338,7 @@
       </c>
     </row>
     <row r="27">
-      <c r="A27" s="17" t="s">
+      <c r="A27" s="19" t="s">
         <v>27</v>
       </c>
       <c r="B27" s="8">
@@ -7343,7 +7346,7 @@
       </c>
     </row>
     <row r="28">
-      <c r="A28" s="17" t="s">
+      <c r="A28" s="19" t="s">
         <v>28</v>
       </c>
       <c r="B28" s="8">
@@ -7373,7 +7376,7 @@
   </sheetViews>
   <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
   <cols>
-    <col customWidth="1" min="1" max="1" width="20.75"/>
+    <col customWidth="1" min="1" max="1" width="25.63"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -7452,7 +7455,7 @@
       <c r="A10" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="B10" s="19">
+      <c r="B10" s="20">
         <v>0.0</v>
       </c>
     </row>
@@ -7473,7 +7476,7 @@
       </c>
     </row>
     <row r="13">
-      <c r="A13" s="11" t="s">
+      <c r="A13" s="10" t="s">
         <v>13</v>
       </c>
       <c r="B13" s="8">
@@ -7521,7 +7524,7 @@
       </c>
     </row>
     <row r="19">
-      <c r="A19" s="14" t="s">
+      <c r="A19" s="15" t="s">
         <v>19</v>
       </c>
       <c r="B19" s="8">
@@ -7529,7 +7532,7 @@
       </c>
     </row>
     <row r="20">
-      <c r="A20" s="14" t="s">
+      <c r="A20" s="15" t="s">
         <v>20</v>
       </c>
       <c r="B20" s="8">
@@ -7545,7 +7548,7 @@
       </c>
     </row>
     <row r="22">
-      <c r="A22" s="15" t="s">
+      <c r="A22" s="16" t="s">
         <v>22</v>
       </c>
       <c r="B22" s="6">
@@ -7553,7 +7556,7 @@
       </c>
     </row>
     <row r="23">
-      <c r="A23" s="16" t="s">
+      <c r="A23" s="17" t="s">
         <v>23</v>
       </c>
       <c r="B23" s="6">
@@ -7577,7 +7580,7 @@
       </c>
     </row>
     <row r="26">
-      <c r="A26" s="17" t="s">
+      <c r="A26" s="18" t="s">
         <v>26</v>
       </c>
       <c r="B26" s="8">
@@ -7585,7 +7588,7 @@
       </c>
     </row>
     <row r="27">
-      <c r="A27" s="17" t="s">
+      <c r="A27" s="19" t="s">
         <v>27</v>
       </c>
       <c r="B27" s="8">
@@ -7593,7 +7596,7 @@
       </c>
     </row>
     <row r="28">
-      <c r="A28" s="17" t="s">
+      <c r="A28" s="19" t="s">
         <v>28</v>
       </c>
       <c r="B28" s="8">

</xml_diff>